<commit_message>
added load function to truck class
</commit_message>
<xml_diff>
--- a/data/WGUPS Distance Table.xlsx
+++ b/data/WGUPS Distance Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\OneDrive\Documents\Study WGU\DSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\PycharmProjects\DSAII\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E91890-1051-44DA-B883-82061B9DE10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA2030D-C68C-49AC-995C-E45A27CD4D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14303" yWindow="-23" windowWidth="21795" windowHeight="12976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,222 +25,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
-  <si>
-    <t>Western Governors University
-4001 South 700 East, 
-Salt Lake City, UT 84107</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve"> HUB</t>
   </si>
   <si>
-    <t>International Peace Gardens
- 1060 Dalton Ave S</t>
+    <t xml:space="preserve"> 1060 Dalton Ave S (84104)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1060 Dalton Ave S
-(84104)</t>
+    <t xml:space="preserve"> 1488 4800 S (84123)</t>
   </si>
   <si>
-    <t>Sugar House Park
- 1330 2100 S</t>
+    <t xml:space="preserve"> 1330 2100 S (84106)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1330 2100 S
-(84106)</t>
+    <t xml:space="preserve"> 177 W Price Ave (84115)</t>
   </si>
   <si>
-    <t>Taylorsville-Bennion Heritage City Gov Off
- 1488 4800 S</t>
+    <t xml:space="preserve"> 195 W Oakland Ave (84115)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1488 4800 S
-(84123)</t>
+    <t xml:space="preserve"> 2010 W 500 S (84104)</t>
   </si>
   <si>
-    <t>Salt Lake City Division of Health Services 
- 177 W Price Ave</t>
+    <t xml:space="preserve"> 2300 Parkway Blvd (84119)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 177 W Price Ave
-(84115)</t>
+    <t xml:space="preserve"> 233 Canyon Rd (84103)</t>
   </si>
   <si>
-    <t>South Salt Lake Public Works
- 195 W Oakland Ave</t>
+    <t xml:space="preserve"> 2530 S 500 E (84106)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 195 W Oakland Ave
-(84115)</t>
+    <t xml:space="preserve"> 2600 Taylorsville Blvd (84118)</t>
   </si>
   <si>
-    <t>Salt Lake City Streets and Sanitation
- 2010 W 500 S</t>
+    <t xml:space="preserve"> 2835 Main St (84115)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2010 W 500 S
-(84104)</t>
+    <t xml:space="preserve"> 300 State St (84103)</t>
   </si>
   <si>
-    <t>Deker Lake
- 2300 Parkway Blvd</t>
+    <t xml:space="preserve"> 3060 Lester St (84119)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2300 Parkway Blvd
-(84119)</t>
+    <t xml:space="preserve"> 3148 S 1100 W (84119)</t>
   </si>
   <si>
-    <t>Salt Lake City Ottinger Hall
- 233 Canyon Rd</t>
+    <t xml:space="preserve"> 3365 S 900 W (84119)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 233 Canyon Rd
-(84103)</t>
+    <t xml:space="preserve"> 3575 W Valley Central Station bus Loop (84119)</t>
   </si>
   <si>
-    <t>Columbus Library
- 2530 S 500 E</t>
+    <t xml:space="preserve"> 3595 Main St (84115)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2530 S 500 E
-(84106)</t>
+    <t xml:space="preserve"> 380 W 2880 S (84115)</t>
   </si>
   <si>
-    <t>Taylorsville City Hall
- 2600 Taylorsville Blvd</t>
+    <t xml:space="preserve"> 410 S State St (84111)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2600 Taylorsville Blvd
-(84118)</t>
+    <t xml:space="preserve"> 4300 S 1300 E (84117)</t>
   </si>
   <si>
-    <t>South Salt Lake Police
- 2835 Main St</t>
+    <t xml:space="preserve"> 4580 S 2300 E (84117)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2835 Main St
-(84115)</t>
+    <t xml:space="preserve"> 5025 State St (84107)</t>
   </si>
   <si>
-    <t>Council Hall
- 300 State St</t>
+    <t xml:space="preserve"> 5100 South 2700 West (84118)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 300 State St
-(84103)</t>
+    <t xml:space="preserve"> 5383 S 900 East #104 (84117)</t>
   </si>
   <si>
-    <t>Redwood Park
- 3060 Lester St</t>
+    <t xml:space="preserve"> 600 E 900 South (84105) </t>
   </si>
   <si>
-    <t xml:space="preserve"> 3060 Lester St
-(84119)</t>
-  </si>
-  <si>
-    <t>Salt Lake County Mental Health
- 3148 S 1100 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3148 S 1100 W
-(84119)</t>
-  </si>
-  <si>
-    <t>Salt Lake County/United Police Dept
- 3365 S 900 W</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3365 S 900 W
-(84119)</t>
-  </si>
-  <si>
-    <t>West Valley Prosecutor
- 3575 W Valley Central Sta bus Loop</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3575 W Valley Central Station bus Loop
-(84119)</t>
-  </si>
-  <si>
-    <t>Housing Auth. of Salt Lake County
- 3595 Main St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3595 Main St
-(84115)</t>
-  </si>
-  <si>
-    <t>Utah DMV Administrative Office
- 380 W 2880 S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 380 W 2880 S
-(84115)</t>
-  </si>
-  <si>
-    <t>Third District Juvenile Court
- 410 S State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 410 S State St
-(84111)</t>
-  </si>
-  <si>
-    <t>Cottonwood Regional Softball Complex
- 4300 S 1300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4300 S 1300 E
-(84117)</t>
-  </si>
-  <si>
-    <t>Holiday City Office
- 4580 S 2300 E</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4580 S 2300 E
-(84117)</t>
-  </si>
-  <si>
-    <t>Murray City Museum
- 5025 State St</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5025 State St
-(84107)</t>
-  </si>
-  <si>
-    <t>Valley Regional Softball Complex
- 5100 South 2700 West</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5100 South 2700 West
-(84118)</t>
-  </si>
-  <si>
-    <t>City Center of Rock Springs
- 5383 South 900 East #104</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5383 S 900 East #104
-(84117)</t>
-  </si>
-  <si>
-    <t>Rice Terrace Pavilion Park
- 600 E 900 South</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 600 E 900 South
-(84105)</t>
-  </si>
-  <si>
-    <t>Wheeler Historic Farm 
- 6351 South 900 East</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6351 South 900 East
-(84121)</t>
+    <t xml:space="preserve"> 6351 South 900 East (84121)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -423,51 +288,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -507,24 +327,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -558,29 +365,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,149 +653,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC28"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="29" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="28" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="177" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="B1" s="5">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="7"/>
     </row>
-    <row r="2" spans="1:29" ht="48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7.2</v>
+      </c>
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="7"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="8"/>
     </row>
-    <row r="3" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
-        <v>7.2</v>
+      <c r="B3" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7.1</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -1032,21 +772,20 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="8"/>
+      <c r="AB3" s="8"/>
     </row>
-    <row r="4" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3.8</v>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6.4</v>
       </c>
       <c r="D4" s="3">
-        <v>7.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -1073,24 +812,23 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="8"/>
+      <c r="AB4" s="8"/>
     </row>
-    <row r="5" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C5" s="3">
         <v>6</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>11</v>
-      </c>
       <c r="D5" s="3">
-        <v>6.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E5" s="3">
-        <v>9.1999999999999993</v>
+        <v>5.6</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -1116,27 +854,26 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="8"/>
+      <c r="AB5" s="8"/>
     </row>
-    <row r="6" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2.2000000000000002</v>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.8</v>
       </c>
       <c r="D6" s="3">
-        <v>6</v>
+        <v>2.8</v>
       </c>
       <c r="E6" s="3">
-        <v>4.4000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="F6" s="3">
-        <v>5.6</v>
+        <v>1.9</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -1161,30 +898,29 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="8"/>
+      <c r="AB6" s="8"/>
     </row>
-    <row r="7" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3.5</v>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>10.9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.6</v>
       </c>
       <c r="D7" s="3">
-        <v>4.8</v>
+        <v>8.6</v>
       </c>
       <c r="E7" s="3">
-        <v>2.8</v>
+        <v>8.6</v>
       </c>
       <c r="F7" s="3">
-        <v>6.9</v>
+        <v>7.9</v>
       </c>
       <c r="G7" s="3">
-        <v>1.9</v>
+        <v>6.3</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
@@ -1208,33 +944,32 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="8"/>
+      <c r="AB7" s="8"/>
     </row>
-    <row r="8" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4">
-        <v>10.9</v>
+    <row r="8" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>8.6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.8</v>
       </c>
       <c r="D8" s="3">
-        <v>1.6</v>
+        <v>6.3</v>
       </c>
       <c r="E8" s="3">
-        <v>8.6</v>
+        <v>4</v>
       </c>
       <c r="F8" s="3">
-        <v>8.6</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G8" s="3">
-        <v>7.9</v>
+        <v>4.3</v>
       </c>
       <c r="H8" s="3">
-        <v>6.3</v>
+        <v>4</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -1257,36 +992,35 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="8"/>
+      <c r="AB8" s="8"/>
     </row>
-    <row r="9" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4">
-        <v>8.6</v>
+    <row r="9" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.8</v>
       </c>
       <c r="D9" s="3">
-        <v>2.8</v>
+        <v>5.3</v>
       </c>
       <c r="E9" s="3">
-        <v>6.3</v>
+        <v>11.1</v>
       </c>
       <c r="F9" s="3">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="G9" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="H9" s="3">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="I9" s="3">
-        <v>4</v>
+        <v>7.7</v>
       </c>
       <c r="J9" s="2">
         <v>0</v>
@@ -1308,39 +1042,38 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="8"/>
+      <c r="AB9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4">
-        <v>7.6</v>
+    <row r="10" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>6.3</v>
       </c>
       <c r="D10" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>7.3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J10" s="3">
         <v>4.8</v>
-      </c>
-      <c r="E10" s="3">
-        <v>5.3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>11.1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="H10" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="I10" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="J10" s="3">
-        <v>7.7</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
@@ -1361,42 +1094,41 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="8"/>
+      <c r="AB10" s="8"/>
     </row>
-    <row r="11" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2.8</v>
+    <row r="11" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7.3</v>
       </c>
       <c r="D11" s="3">
-        <v>6.3</v>
+        <v>10.4</v>
       </c>
       <c r="E11" s="3">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>7.3</v>
+        <v>6.5</v>
       </c>
       <c r="G11" s="3">
-        <v>2.6</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H11" s="3">
-        <v>1.5</v>
+        <v>8.6</v>
       </c>
       <c r="I11" s="3">
-        <v>8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J11" s="3">
-        <v>9.3000000000000007</v>
+        <v>11.9</v>
       </c>
       <c r="K11" s="3">
-        <v>4.8</v>
+        <v>9.4</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
@@ -1416,45 +1148,44 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="8"/>
+      <c r="AB11" s="8"/>
     </row>
-    <row r="12" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4">
+    <row r="12" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="3">
         <v>6.4</v>
       </c>
-      <c r="D12" s="3">
+      <c r="F12" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="H12" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="J12" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L12" s="3">
         <v>7.3</v>
-      </c>
-      <c r="E12" s="3">
-        <v>10.4</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="H12" s="3">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="I12" s="3">
-        <v>8.6</v>
-      </c>
-      <c r="J12" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="K12" s="3">
-        <v>11.9</v>
-      </c>
-      <c r="L12" s="3">
-        <v>9.4</v>
       </c>
       <c r="M12" s="2">
         <v>0</v>
@@ -1473,48 +1204,47 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="8"/>
+      <c r="AB12" s="8"/>
     </row>
-    <row r="13" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4">
-        <v>3.2</v>
+    <row r="13" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4.8</v>
       </c>
       <c r="D13" s="3">
         <v>5.3</v>
       </c>
       <c r="E13" s="3">
-        <v>3</v>
+        <v>11.1</v>
       </c>
       <c r="F13" s="3">
-        <v>6.4</v>
+        <v>7.5</v>
       </c>
       <c r="G13" s="3">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="H13" s="3">
-        <v>0.8</v>
+        <v>4.2</v>
       </c>
       <c r="I13" s="3">
-        <v>6.9</v>
+        <v>7.7</v>
       </c>
       <c r="J13" s="3">
-        <v>4.8</v>
+        <v>0.6</v>
       </c>
       <c r="K13" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="L13" s="3">
+        <v>12</v>
+      </c>
+      <c r="M13" s="3">
         <v>4.7</v>
-      </c>
-      <c r="L13" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M13" s="3">
-        <v>7.3</v>
       </c>
       <c r="N13" s="2">
         <v>0</v>
@@ -1532,51 +1262,50 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="8"/>
+      <c r="AB13" s="8"/>
     </row>
-    <row r="14" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="4">
+    <row r="14" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="J14" s="3">
         <v>7.6</v>
       </c>
-      <c r="D14" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="E14" s="3">
-        <v>5.3</v>
-      </c>
-      <c r="F14" s="3">
-        <v>11.1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="H14" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="I14" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="J14" s="3">
-        <v>7.7</v>
-      </c>
       <c r="K14" s="3">
-        <v>0.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="L14" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="M14" s="3">
-        <v>12</v>
+        <v>3.5</v>
       </c>
       <c r="N14" s="3">
-        <v>4.7</v>
+        <v>7.3</v>
       </c>
       <c r="O14" s="2">
         <v>0</v>
@@ -1593,54 +1322,53 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="8"/>
+      <c r="AB14" s="8"/>
     </row>
-    <row r="15" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="4">
+    <row r="15" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="E15" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <v>8</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="J15" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="L15" s="3">
         <v>5.2</v>
       </c>
-      <c r="D15" s="3">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="F15" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="G15" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="H15" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="I15" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="J15" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="K15" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="L15" s="3">
-        <v>4.5999999999999996</v>
-      </c>
       <c r="M15" s="3">
-        <v>4.9000000000000004</v>
+        <v>2.6</v>
       </c>
       <c r="N15" s="3">
-        <v>3.5</v>
+        <v>7.8</v>
       </c>
       <c r="O15" s="3">
-        <v>7.3</v>
+        <v>1.3</v>
       </c>
       <c r="P15" s="2">
         <v>0</v>
@@ -1656,57 +1384,56 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="8"/>
+      <c r="AB15" s="8"/>
     </row>
-    <row r="16" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4">
+    <row r="16" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3.66112816434</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="E16" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D16" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E16" s="3">
-        <v>5.6</v>
-      </c>
       <c r="F16" s="3">
-        <v>4.3</v>
+        <v>2.7</v>
       </c>
       <c r="G16" s="3">
-        <v>2.4</v>
+        <v>3.8</v>
       </c>
       <c r="H16" s="3">
-        <v>3</v>
+        <v>5.8</v>
       </c>
       <c r="I16" s="3">
-        <v>8</v>
+        <v>3.4</v>
       </c>
       <c r="J16" s="3">
-        <v>3.3</v>
+        <v>6.6</v>
       </c>
       <c r="K16" s="3">
-        <v>7.8</v>
+        <v>4</v>
       </c>
       <c r="L16" s="3">
-        <v>3.7</v>
+        <v>5.4</v>
       </c>
       <c r="M16" s="3">
-        <v>5.2</v>
+        <v>2.9</v>
       </c>
       <c r="N16" s="3">
-        <v>2.6</v>
+        <v>6.6</v>
       </c>
       <c r="O16" s="3">
-        <v>7.8</v>
+        <v>1.5</v>
       </c>
       <c r="P16" s="3">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="Q16" s="2">
         <v>0</v>
@@ -1721,60 +1448,59 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="8"/>
+      <c r="AB16" s="8"/>
     </row>
-    <row r="17" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="4">
-        <v>3.66112816434</v>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="C17" s="3">
+        <v>7.4</v>
       </c>
       <c r="D17" s="3">
-        <v>4.5</v>
+        <v>5.7</v>
       </c>
       <c r="E17" s="3">
-        <v>5.8</v>
+        <v>7.2</v>
       </c>
       <c r="F17" s="3">
-        <v>4.4000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="G17" s="3">
-        <v>2.7</v>
+        <v>5.7</v>
       </c>
       <c r="H17" s="3">
-        <v>3.8</v>
+        <v>7.2</v>
       </c>
       <c r="I17" s="3">
-        <v>5.8</v>
+        <v>3.1</v>
       </c>
       <c r="J17" s="3">
-        <v>3.4</v>
+        <v>7.2</v>
       </c>
       <c r="K17" s="3">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="L17" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="N17" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="O17" s="3">
         <v>4</v>
       </c>
-      <c r="M17" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="N17" s="3">
-        <v>2.9</v>
-      </c>
-      <c r="O17" s="3">
-        <v>6.6</v>
-      </c>
       <c r="P17" s="3">
-        <v>1.5</v>
+        <v>6.4</v>
       </c>
       <c r="Q17" s="3">
-        <v>0.6</v>
+        <v>5.6</v>
       </c>
       <c r="R17" s="2">
         <v>0</v>
@@ -1788,63 +1514,62 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="8"/>
+      <c r="AB17" s="8"/>
     </row>
-    <row r="18" spans="1:29" ht="48" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="4">
-        <v>7.6</v>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>6</v>
       </c>
       <c r="D18" s="3">
-        <v>7.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E18" s="3">
-        <v>5.7</v>
+        <v>5.3</v>
       </c>
       <c r="F18" s="3">
-        <v>7.2</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="3">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="H18" s="3">
-        <v>5.7</v>
+        <v>7.7</v>
       </c>
       <c r="I18" s="3">
-        <v>7.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="J18" s="3">
-        <v>3.1</v>
+        <v>5.9</v>
       </c>
       <c r="K18" s="3">
-        <v>7.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L18" s="3">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="M18" s="3">
-        <v>8.1</v>
+        <v>1.2</v>
       </c>
       <c r="N18" s="3">
-        <v>6.3</v>
+        <v>5.9</v>
       </c>
       <c r="O18" s="3">
-        <v>7.2</v>
+        <v>3.2</v>
       </c>
       <c r="P18" s="3">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="Q18" s="3">
-        <v>6.4</v>
+        <v>1.6</v>
       </c>
       <c r="R18" s="3">
-        <v>5.6</v>
+        <v>7.1</v>
       </c>
       <c r="S18" s="2">
         <v>0</v>
@@ -1857,66 +1582,65 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="8"/>
+      <c r="AB18" s="8"/>
     </row>
-    <row r="19" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="4">
-        <v>2</v>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="C19" s="3">
+        <v>5</v>
       </c>
       <c r="D19" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E19" s="3">
         <v>6</v>
       </c>
-      <c r="E19" s="3">
-        <v>4.0999999999999996</v>
-      </c>
       <c r="F19" s="3">
-        <v>5.3</v>
+        <v>1.7</v>
       </c>
       <c r="G19" s="3">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H19" s="3">
-        <v>1.9</v>
+        <v>6.6</v>
       </c>
       <c r="I19" s="3">
-        <v>7.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J19" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.4</v>
       </c>
       <c r="K19" s="3">
-        <v>5.9</v>
+        <v>1.8</v>
       </c>
       <c r="L19" s="3">
-        <v>2.2999999999999998</v>
+        <v>6.9</v>
       </c>
       <c r="M19" s="3">
-        <v>6.2</v>
+        <v>1</v>
       </c>
       <c r="N19" s="3">
-        <v>1.2</v>
+        <v>5.4</v>
       </c>
       <c r="O19" s="3">
-        <v>5.9</v>
+        <v>3</v>
       </c>
       <c r="P19" s="3">
-        <v>3.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q19" s="3">
-        <v>2.4</v>
+        <v>1.7</v>
       </c>
       <c r="R19" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="S19" s="3">
         <v>1.6</v>
-      </c>
-      <c r="S19" s="3">
-        <v>7.1</v>
       </c>
       <c r="T19" s="2">
         <v>0</v>
@@ -1928,69 +1652,68 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="8"/>
+      <c r="AB19" s="8"/>
     </row>
-    <row r="20" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="4">
-        <v>3.6</v>
+    <row r="20" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4.8</v>
       </c>
       <c r="D20" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="E20" s="3">
-        <v>3.6</v>
+        <v>10.6</v>
       </c>
       <c r="F20" s="3">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="G20" s="3">
-        <v>1.7</v>
+        <v>3.5</v>
       </c>
       <c r="H20" s="3">
-        <v>1.1000000000000001</v>
+        <v>3.2</v>
       </c>
       <c r="I20" s="3">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="J20" s="3">
-        <v>4.5999999999999996</v>
+        <v>1</v>
       </c>
       <c r="K20" s="3">
-        <v>5.4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="L20" s="3">
-        <v>1.8</v>
+        <v>11.5</v>
       </c>
       <c r="M20" s="3">
-        <v>6.9</v>
+        <v>3.7</v>
       </c>
       <c r="N20" s="3">
         <v>1</v>
       </c>
       <c r="O20" s="3">
-        <v>5.4</v>
+        <v>6.9</v>
       </c>
       <c r="P20" s="3">
-        <v>3</v>
+        <v>6.8</v>
       </c>
       <c r="Q20" s="3">
-        <v>2.2000000000000002</v>
+        <v>6.4</v>
       </c>
       <c r="R20" s="3">
-        <v>1.7</v>
+        <v>7.2</v>
       </c>
       <c r="S20" s="3">
-        <v>6.1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="T20" s="3">
-        <v>1.6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="U20" s="2">
         <v>0</v>
@@ -2001,72 +1724,71 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="8"/>
+      <c r="AB20" s="8"/>
     </row>
-    <row r="21" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="4">
-        <v>6.5</v>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="C21" s="3">
+        <v>9.5</v>
       </c>
       <c r="D21" s="3">
-        <v>4.8</v>
+        <v>3.3</v>
       </c>
       <c r="E21" s="3">
-        <v>4.3</v>
+        <v>5.9</v>
       </c>
       <c r="F21" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H21" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="I21" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="L21" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="M21" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N21" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="O21" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="P21" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R21" s="3">
         <v>10.6</v>
       </c>
-      <c r="G21" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="H21" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I21" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="J21" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="K21" s="3">
-        <v>1</v>
-      </c>
-      <c r="L21" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="M21" s="3">
-        <v>11.5</v>
-      </c>
-      <c r="N21" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="O21" s="3">
-        <v>1</v>
-      </c>
-      <c r="P21" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="R21" s="3">
-        <v>6.4</v>
-      </c>
       <c r="S21" s="3">
-        <v>7.2</v>
+        <v>3</v>
       </c>
       <c r="T21" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="U21" s="3">
-        <v>4.4000000000000004</v>
+        <v>7.5</v>
       </c>
       <c r="V21" s="2">
         <v>0</v>
@@ -2076,75 +1798,74 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="8"/>
+      <c r="AB21" s="8"/>
     </row>
-    <row r="22" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1.9</v>
+    <row r="22" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="C22" s="3">
+        <v>10.9</v>
       </c>
       <c r="D22" s="3">
-        <v>9.5</v>
+        <v>5</v>
       </c>
       <c r="E22" s="3">
-        <v>3.3</v>
+        <v>7.4</v>
       </c>
       <c r="F22" s="3">
-        <v>5.9</v>
+        <v>5.2</v>
       </c>
       <c r="G22" s="3">
-        <v>3.2</v>
+        <v>6.9</v>
       </c>
       <c r="H22" s="3">
-        <v>4.9000000000000004</v>
+        <v>12.7</v>
       </c>
       <c r="I22" s="3">
-        <v>11.2</v>
+        <v>10.4</v>
       </c>
       <c r="J22" s="3">
-        <v>8.1</v>
+        <v>10.3</v>
       </c>
       <c r="K22" s="3">
-        <v>8.5</v>
+        <v>5.8</v>
       </c>
       <c r="L22" s="3">
-        <v>3.8</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="M22" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="N22" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="O22" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="P22" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="Q22" s="3">
         <v>6.9</v>
       </c>
-      <c r="N22" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="O22" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="P22" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="Q22" s="3">
-        <v>5.3</v>
-      </c>
       <c r="R22" s="3">
-        <v>4.9000000000000004</v>
+        <v>12</v>
       </c>
       <c r="S22" s="3">
-        <v>10.6</v>
+        <v>5</v>
       </c>
       <c r="T22" s="3">
-        <v>3</v>
+        <v>6.6</v>
       </c>
       <c r="U22" s="3">
-        <v>4.5999999999999996</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="V22" s="3">
-        <v>7.5</v>
+        <v>2</v>
       </c>
       <c r="W22" s="2">
         <v>0</v>
@@ -2153,78 +1874,77 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="8"/>
+      <c r="AB22" s="8"/>
     </row>
-    <row r="23" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="4">
+    <row r="23" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="C23" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D23" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="H23" s="3">
+        <v>10</v>
+      </c>
+      <c r="I23" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="J23" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M23" s="3">
         <v>3.4</v>
       </c>
-      <c r="D23" s="3">
-        <v>10.9</v>
-      </c>
-      <c r="E23" s="3">
-        <v>5</v>
-      </c>
-      <c r="F23" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="G23" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="H23" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="I23" s="3">
-        <v>12.7</v>
-      </c>
-      <c r="J23" s="3">
-        <v>10.4</v>
-      </c>
-      <c r="K23" s="3">
-        <v>10.3</v>
-      </c>
-      <c r="L23" s="3">
-        <v>5.8</v>
-      </c>
-      <c r="M23" s="3">
-        <v>8.3000000000000007</v>
-      </c>
       <c r="N23" s="3">
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="O23" s="3">
-        <v>10.3</v>
+        <v>5.5</v>
       </c>
       <c r="P23" s="3">
-        <v>8.1999999999999993</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="Q23" s="3">
-        <v>7.4</v>
+        <v>4.2</v>
       </c>
       <c r="R23" s="3">
-        <v>6.9</v>
+        <v>9.4</v>
       </c>
       <c r="S23" s="3">
-        <v>12</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="T23" s="3">
-        <v>5</v>
+        <v>3.9</v>
       </c>
       <c r="U23" s="3">
-        <v>6.6</v>
+        <v>6.8</v>
       </c>
       <c r="V23" s="3">
-        <v>9.3000000000000007</v>
+        <v>2.9</v>
       </c>
       <c r="W23" s="3">
-        <v>2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="X23" s="2">
         <v>0</v>
@@ -2232,431 +1952,337 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="8"/>
+      <c r="AB23" s="8"/>
     </row>
-    <row r="24" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="4">
-        <v>2.4</v>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="C24" s="3">
+        <v>6.9</v>
       </c>
       <c r="D24" s="3">
-        <v>8.3000000000000007</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="E24" s="3">
-        <v>6.1</v>
+        <v>0.6</v>
       </c>
       <c r="F24" s="3">
-        <v>4.7</v>
+        <v>6</v>
       </c>
       <c r="G24" s="3">
-        <v>2.5</v>
+        <v>9</v>
       </c>
       <c r="H24" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I24" s="3">
         <v>4.2</v>
       </c>
-      <c r="I24" s="3">
-        <v>10</v>
-      </c>
       <c r="J24" s="3">
-        <v>7.8</v>
+        <v>11.5</v>
       </c>
       <c r="K24" s="3">
         <v>7.8</v>
       </c>
       <c r="L24" s="3">
-        <v>4.3</v>
+        <v>0.4</v>
       </c>
       <c r="M24" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.9</v>
       </c>
       <c r="N24" s="3">
-        <v>3.4</v>
+        <v>11.5</v>
       </c>
       <c r="O24" s="3">
-        <v>7.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="P24" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="R24" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="S24" s="3">
         <v>5.5</v>
       </c>
-      <c r="Q24" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="R24" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="S24" s="3">
-        <v>9.4</v>
-      </c>
       <c r="T24" s="3">
-        <v>2.2999999999999998</v>
+        <v>6.5</v>
       </c>
       <c r="U24" s="3">
-        <v>3.9</v>
+        <v>11.4</v>
       </c>
       <c r="V24" s="3">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="W24" s="3">
-        <v>2.9</v>
+        <v>7.9</v>
       </c>
       <c r="X24" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="Y24" s="2">
         <v>0</v>
       </c>
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
-      <c r="AC24" s="8"/>
+      <c r="AB24" s="8"/>
     </row>
-    <row r="25" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="4">
+    <row r="25" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="C25" s="3">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="E25" s="3">
         <v>6.4</v>
       </c>
-      <c r="D25" s="3">
-        <v>6.9</v>
-      </c>
-      <c r="E25" s="3">
-        <v>9.6999999999999993</v>
-      </c>
       <c r="F25" s="3">
-        <v>0.6</v>
+        <v>4.2</v>
       </c>
       <c r="G25" s="3">
-        <v>6</v>
+        <v>5.9</v>
       </c>
       <c r="H25" s="3">
-        <v>9</v>
+        <v>11.7</v>
       </c>
       <c r="I25" s="3">
-        <v>8.1999999999999993</v>
+        <v>9.5</v>
       </c>
       <c r="J25" s="3">
-        <v>4.2</v>
+        <v>9.5</v>
       </c>
       <c r="K25" s="3">
-        <v>11.5</v>
+        <v>4.8</v>
       </c>
       <c r="L25" s="3">
-        <v>7.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="M25" s="3">
-        <v>0.4</v>
+        <v>5.2</v>
       </c>
       <c r="N25" s="3">
-        <v>6.9</v>
+        <v>9.5</v>
       </c>
       <c r="O25" s="3">
-        <v>11.5</v>
+        <v>7.2</v>
       </c>
       <c r="P25" s="3">
-        <v>4.4000000000000004</v>
+        <v>6.3</v>
       </c>
       <c r="Q25" s="3">
-        <v>4.8</v>
+        <v>5.9</v>
       </c>
       <c r="R25" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="S25" s="3">
+        <v>4</v>
+      </c>
+      <c r="T25" s="3">
         <v>5.6</v>
       </c>
-      <c r="S25" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="T25" s="3">
-        <v>5.5</v>
-      </c>
       <c r="U25" s="3">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="V25" s="3">
-        <v>11.4</v>
+        <v>2.8</v>
       </c>
       <c r="W25" s="3">
-        <v>6.4</v>
+        <v>3.4</v>
       </c>
       <c r="X25" s="3">
-        <v>7.9</v>
+        <v>1.7</v>
       </c>
       <c r="Y25" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
       <c r="Z25" s="2">
         <v>0</v>
       </c>
       <c r="AA25" s="3"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="8"/>
+      <c r="AB25" s="8"/>
     </row>
-    <row r="26" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2.4</v>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4.4000000000000004</v>
       </c>
       <c r="D26" s="3">
-        <v>10</v>
+        <v>2.8</v>
       </c>
       <c r="E26" s="3">
-        <v>6.1</v>
+        <v>10.1</v>
       </c>
       <c r="F26" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="H26" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I26" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="J26" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="K26" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="L26" s="3">
+        <v>11</v>
+      </c>
+      <c r="M26" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="N26" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="O26" s="3">
         <v>6.4</v>
       </c>
-      <c r="G26" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="H26" s="3">
-        <v>5.9</v>
-      </c>
-      <c r="I26" s="3">
-        <v>11.7</v>
-      </c>
-      <c r="J26" s="3">
-        <v>9.5</v>
-      </c>
-      <c r="K26" s="3">
-        <v>9.5</v>
-      </c>
-      <c r="L26" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="M26" s="3">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="N26" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="O26" s="3">
-        <v>9.5</v>
-      </c>
       <c r="P26" s="3">
-        <v>7.2</v>
+        <v>6.5</v>
       </c>
       <c r="Q26" s="3">
-        <v>6.3</v>
+        <v>5.7</v>
       </c>
       <c r="R26" s="3">
-        <v>5.9</v>
+        <v>6.2</v>
       </c>
       <c r="S26" s="3">
-        <v>11.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="T26" s="3">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="U26" s="3">
-        <v>5.6</v>
+        <v>1.8</v>
       </c>
       <c r="V26" s="3">
-        <v>8.5</v>
+        <v>6</v>
       </c>
       <c r="W26" s="3">
-        <v>2.8</v>
+        <v>7.9</v>
       </c>
       <c r="X26" s="3">
-        <v>3.4</v>
+        <v>6.8</v>
       </c>
       <c r="Y26" s="3">
-        <v>1.7</v>
+        <v>10.6</v>
       </c>
       <c r="Z26" s="3">
-        <v>5.4</v>
+        <v>7</v>
       </c>
       <c r="AA26" s="2">
         <v>0</v>
       </c>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="8"/>
+      <c r="AB26" s="8"/>
     </row>
-    <row r="27" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="4">
-        <v>5</v>
-      </c>
-      <c r="D27" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E27" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="F27" s="3">
+    <row r="27" spans="1:28" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9">
+        <v>3.6</v>
+      </c>
+      <c r="C27" s="10">
+        <v>13</v>
+      </c>
+      <c r="D27" s="10">
+        <v>7.4</v>
+      </c>
+      <c r="E27" s="10">
         <v>10.1</v>
       </c>
-      <c r="G27" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="H27" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="I27" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="J27" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="K27" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="L27" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="M27" s="3">
-        <v>11</v>
-      </c>
-      <c r="N27" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="O27" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="P27" s="3">
+      <c r="F27" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="G27" s="10">
+        <v>7.2</v>
+      </c>
+      <c r="H27" s="10">
+        <v>14.2</v>
+      </c>
+      <c r="I27" s="10">
+        <v>10.7</v>
+      </c>
+      <c r="J27" s="10">
+        <v>14.1</v>
+      </c>
+      <c r="K27" s="10">
+        <v>6</v>
+      </c>
+      <c r="L27" s="10">
+        <v>6.8</v>
+      </c>
+      <c r="M27" s="10">
         <v>6.4</v>
       </c>
-      <c r="Q27" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="R27" s="3">
-        <v>5.7</v>
-      </c>
-      <c r="S27" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="T27" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="U27" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="V27" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="W27" s="3">
-        <v>6</v>
-      </c>
-      <c r="X27" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="Y27" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="Z27" s="3">
-        <v>10.6</v>
-      </c>
-      <c r="AA27" s="3">
-        <v>7</v>
-      </c>
-      <c r="AB27" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="8"/>
-    </row>
-    <row r="28" spans="1:29" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="9">
-        <v>3.6</v>
-      </c>
-      <c r="D28" s="10">
-        <v>13</v>
-      </c>
-      <c r="E28" s="10">
-        <v>7.4</v>
-      </c>
-      <c r="F28" s="10">
-        <v>10.1</v>
-      </c>
-      <c r="G28" s="10">
-        <v>5.5</v>
-      </c>
-      <c r="H28" s="10">
-        <v>7.2</v>
-      </c>
-      <c r="I28" s="10">
-        <v>14.2</v>
-      </c>
-      <c r="J28" s="10">
-        <v>10.7</v>
-      </c>
-      <c r="K28" s="10">
+      <c r="N27" s="10">
         <v>14.1</v>
       </c>
-      <c r="L28" s="10">
-        <v>6</v>
-      </c>
-      <c r="M28" s="10">
-        <v>6.8</v>
-      </c>
-      <c r="N28" s="10">
-        <v>6.4</v>
-      </c>
-      <c r="O28" s="10">
-        <v>14.1</v>
-      </c>
-      <c r="P28" s="10">
+      <c r="O27" s="10">
         <v>10.5</v>
       </c>
-      <c r="Q28" s="10">
+      <c r="P27" s="10">
         <v>8.8000000000000007</v>
       </c>
-      <c r="R28" s="10">
+      <c r="Q27" s="10">
         <v>8.4</v>
       </c>
-      <c r="S28" s="10">
+      <c r="R27" s="10">
         <v>13.6</v>
       </c>
-      <c r="T28" s="10">
+      <c r="S27" s="10">
         <v>5.2</v>
       </c>
-      <c r="U28" s="10">
+      <c r="T27" s="10">
         <v>6.9</v>
       </c>
-      <c r="V28" s="10">
+      <c r="U27" s="10">
         <v>13.1</v>
       </c>
-      <c r="W28" s="10">
+      <c r="V27" s="10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="X28" s="10">
+      <c r="W27" s="10">
         <v>4.7</v>
       </c>
-      <c r="Y28" s="10">
+      <c r="X27" s="10">
         <v>3.1</v>
       </c>
-      <c r="Z28" s="10">
+      <c r="Y27" s="10">
         <v>7.8</v>
       </c>
-      <c r="AA28" s="10">
+      <c r="Z27" s="10">
         <v>1.3</v>
       </c>
-      <c r="AB28" s="10">
+      <c r="AA27" s="10">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AC28" s="11">
+      <c r="AB27" s="11">
         <v>0</v>
       </c>
     </row>
@@ -2667,15 +2293,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3185,6 +2802,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3235,14 +2861,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3258,6 +2876,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
made function that returns all possible locations and distances from current in a dictionary
</commit_message>
<xml_diff>
--- a/data/WGUPS Distance Table.xlsx
+++ b/data/WGUPS Distance Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\PycharmProjects\DSAII\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA2030D-C68C-49AC-995C-E45A27CD4D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E84C1E9-D498-48DA-A7BF-C629DE07A583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-23" windowWidth="21795" windowHeight="12976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,82 +30,82 @@
     <t xml:space="preserve"> HUB</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1060 Dalton Ave S (84104)</t>
+    <t xml:space="preserve"> 1060 Dalton Ave S</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1488 4800 S (84123)</t>
+    <t xml:space="preserve"> 1330 2100 S</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1330 2100 S (84106)</t>
+    <t xml:space="preserve"> 1488 4800 S</t>
   </si>
   <si>
-    <t xml:space="preserve"> 177 W Price Ave (84115)</t>
+    <t xml:space="preserve"> 177 W Price Ave</t>
   </si>
   <si>
-    <t xml:space="preserve"> 195 W Oakland Ave (84115)</t>
+    <t xml:space="preserve"> 195 W Oakland Ave</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2010 W 500 S (84104)</t>
+    <t xml:space="preserve"> 2010 W 500 S</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2300 Parkway Blvd (84119)</t>
+    <t xml:space="preserve"> 2300 Parkway Blvd</t>
   </si>
   <si>
-    <t xml:space="preserve"> 233 Canyon Rd (84103)</t>
+    <t xml:space="preserve"> 233 Canyon Rd</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2530 S 500 E (84106)</t>
+    <t xml:space="preserve"> 2530 S 500 E</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2600 Taylorsville Blvd (84118)</t>
+    <t xml:space="preserve"> 2600 Taylorsville Blvd</t>
   </si>
   <si>
-    <t xml:space="preserve"> 2835 Main St (84115)</t>
+    <t xml:space="preserve"> 2835 Main St</t>
   </si>
   <si>
-    <t xml:space="preserve"> 300 State St (84103)</t>
+    <t xml:space="preserve"> 300 State St</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3060 Lester St (84119)</t>
+    <t xml:space="preserve"> 3060 Lester St</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3148 S 1100 W (84119)</t>
+    <t xml:space="preserve"> 3148 S 1100 W</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3365 S 900 W (84119)</t>
+    <t xml:space="preserve"> 3365 S 900 W</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3575 W Valley Central Station bus Loop (84119)</t>
+    <t xml:space="preserve"> 3575 W Valley Central Station bus Loop</t>
   </si>
   <si>
-    <t xml:space="preserve"> 3595 Main St (84115)</t>
+    <t xml:space="preserve"> 3595 Main St</t>
   </si>
   <si>
-    <t xml:space="preserve"> 380 W 2880 S (84115)</t>
+    <t xml:space="preserve"> 380 W 2880 S</t>
   </si>
   <si>
-    <t xml:space="preserve"> 410 S State St (84111)</t>
+    <t xml:space="preserve"> 410 S State St</t>
   </si>
   <si>
-    <t xml:space="preserve"> 4300 S 1300 E (84117)</t>
+    <t xml:space="preserve"> 4300 S 1300 E</t>
   </si>
   <si>
-    <t xml:space="preserve"> 4580 S 2300 E (84117)</t>
+    <t xml:space="preserve"> 4580 S 2300 E</t>
   </si>
   <si>
-    <t xml:space="preserve"> 5025 State St (84107)</t>
+    <t xml:space="preserve"> 5025 State St</t>
   </si>
   <si>
-    <t xml:space="preserve"> 5100 South 2700 West (84118)</t>
+    <t xml:space="preserve"> 5100 South 2700 West</t>
   </si>
   <si>
-    <t xml:space="preserve"> 5383 S 900 East #104 (84117)</t>
+    <t xml:space="preserve"> 5383 S 900 East #104</t>
   </si>
   <si>
-    <t xml:space="preserve"> 600 E 900 South (84105) </t>
+    <t xml:space="preserve"> 600 E 900 South</t>
   </si>
   <si>
-    <t xml:space="preserve"> 6351 South 900 East (84121)</t>
+    <t xml:space="preserve"> 6351 South 900 East</t>
   </si>
 </sst>
 </file>
@@ -153,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -327,11 +327,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -371,6 +402,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -653,27 +693,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="28" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="29" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="15"/>
+      <c r="C1" s="5">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -698,19 +739,22 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
       <c r="AA1" s="6"/>
-      <c r="AB1" s="7"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="7"/>
     </row>
-    <row r="2" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="16">
+        <v>84104</v>
+      </c>
+      <c r="C2" s="4">
         <v>7.2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -734,22 +778,25 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
-      <c r="AB2" s="8"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="8"/>
     </row>
-    <row r="3" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16">
+        <v>84106</v>
+      </c>
+      <c r="C3" s="4">
         <v>3.8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>7.1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -772,25 +819,28 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="8"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="8"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16">
+        <v>84123</v>
+      </c>
+      <c r="C4" s="4">
         <v>11</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>6.4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -812,28 +862,31 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="8"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="8"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="16">
+        <v>84115</v>
+      </c>
+      <c r="C5" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>6</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>5.6</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -854,31 +907,34 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="8"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="16">
+        <v>84155</v>
+      </c>
+      <c r="C6" s="4">
         <v>3.5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>4.8</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>2.8</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>6.9</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>1.9</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -898,34 +954,37 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="8"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="8"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="16">
+        <v>84104</v>
+      </c>
+      <c r="C7" s="4">
         <v>10.9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>1.6</v>
-      </c>
-      <c r="D7" s="3">
-        <v>8.6</v>
       </c>
       <c r="E7" s="3">
         <v>8.6</v>
       </c>
       <c r="F7" s="3">
+        <v>8.6</v>
+      </c>
+      <c r="G7" s="3">
         <v>7.9</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>6.3</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -944,37 +1003,40 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="8"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="16">
+        <v>84119</v>
+      </c>
+      <c r="C8" s="4">
         <v>8.6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>2.8</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>6.3</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>4</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>4.3</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>4</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>0</v>
       </c>
-      <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -992,40 +1054,43 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="8"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="8"/>
     </row>
-    <row r="9" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="16">
+        <v>84103</v>
+      </c>
+      <c r="C9" s="4">
         <v>7.6</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>4.8</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>5.3</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>11.1</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>7.5</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>4.5</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>4.2</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>7.7</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>0</v>
       </c>
-      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -1042,43 +1107,46 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="8"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="16">
+        <v>84106</v>
+      </c>
+      <c r="C10" s="4">
         <v>2.8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>6.3</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>1.6</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>7.3</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>2.6</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>1.5</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>8</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>4.8</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -1094,46 +1162,49 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="8"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="8"/>
     </row>
-    <row r="11" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="16">
+        <v>84118</v>
+      </c>
+      <c r="C11" s="4">
         <v>6.4</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>7.3</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>10.4</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>6.5</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>8.6999999999999993</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>8.6</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>11.9</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>9.4</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>0</v>
       </c>
-      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -1148,49 +1219,52 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="8"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="8"/>
     </row>
-    <row r="12" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="16">
+        <v>84115</v>
+      </c>
+      <c r="C12" s="4">
         <v>3.2</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>5.3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>3</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>6.4</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>1.5</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>0.8</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>6.9</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>4.8</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>4.7</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <v>7.3</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>0</v>
       </c>
-      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1204,52 +1278,55 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="8"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="8"/>
     </row>
-    <row r="13" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="16">
+        <v>84103</v>
+      </c>
+      <c r="C13" s="4">
         <v>7.6</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>4.8</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>5.3</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>11.1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>7.5</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>4.5</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>4.2</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>7.7</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>0.6</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <v>12</v>
       </c>
-      <c r="M13" s="3">
+      <c r="N13" s="3">
         <v>4.7</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>0</v>
       </c>
-      <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -1262,55 +1339,58 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3"/>
-      <c r="AB13" s="8"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="8"/>
     </row>
-    <row r="14" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="16">
+        <v>84119</v>
+      </c>
+      <c r="C14" s="4">
         <v>5.2</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>3</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>6.5</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>3.9</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>3.2</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>3.9</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>4.2</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>1.6</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>7.6</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M14" s="3">
+      <c r="N14" s="3">
         <v>3.5</v>
       </c>
-      <c r="N14" s="3">
+      <c r="O14" s="3">
         <v>7.3</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>0</v>
       </c>
-      <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
@@ -1322,58 +1402,61 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
-      <c r="AB14" s="8"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="8"/>
     </row>
-    <row r="15" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="16">
+        <v>84119</v>
+      </c>
+      <c r="C15" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>5.6</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>4.3</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>2.4</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>3</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>8</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>3.3</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>7.8</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L15" s="3">
         <v>3.7</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <v>5.2</v>
       </c>
-      <c r="M15" s="3">
+      <c r="N15" s="3">
         <v>2.6</v>
       </c>
-      <c r="N15" s="3">
+      <c r="O15" s="3">
         <v>7.8</v>
       </c>
-      <c r="O15" s="3">
+      <c r="P15" s="3">
         <v>1.3</v>
       </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>0</v>
       </c>
-      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -1384,61 +1467,64 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="8"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="8"/>
     </row>
-    <row r="16" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="16">
+        <v>84119</v>
+      </c>
+      <c r="C16" s="4">
         <v>3.66112816434</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>4.5</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>5.8</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>2.7</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>3.8</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>5.8</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>3.4</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>6.6</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <v>4</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <v>5.4</v>
       </c>
-      <c r="M16" s="3">
+      <c r="N16" s="3">
         <v>2.9</v>
       </c>
-      <c r="N16" s="3">
+      <c r="O16" s="3">
         <v>6.6</v>
       </c>
-      <c r="O16" s="3">
+      <c r="P16" s="3">
         <v>1.5</v>
       </c>
-      <c r="P16" s="3">
+      <c r="Q16" s="3">
         <v>0.6</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
         <v>0</v>
       </c>
-      <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
@@ -1448,64 +1534,67 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="8"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="8"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="16">
+        <v>84119</v>
+      </c>
+      <c r="C17" s="4">
         <v>7.6</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>7.4</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>5.7</v>
       </c>
-      <c r="E17" s="3">
+      <c r="F17" s="3">
         <v>7.2</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>1.4</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>5.7</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>7.2</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>3.1</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>7.2</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L17" s="3">
         <v>6.7</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M17" s="3">
         <v>8.1</v>
       </c>
-      <c r="M17" s="3">
+      <c r="N17" s="3">
         <v>6.3</v>
       </c>
-      <c r="N17" s="3">
+      <c r="O17" s="3">
         <v>7.2</v>
       </c>
-      <c r="O17" s="3">
+      <c r="P17" s="3">
         <v>4</v>
       </c>
-      <c r="P17" s="3">
+      <c r="Q17" s="3">
         <v>6.4</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="R17" s="3">
         <v>5.6</v>
       </c>
-      <c r="R17" s="2">
+      <c r="S17" s="2">
         <v>0</v>
       </c>
-      <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -1514,67 +1603,70 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="8"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="8"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="16">
+        <v>84115</v>
+      </c>
+      <c r="C18" s="4">
         <v>2</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <v>6</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E18" s="3">
+      <c r="F18" s="3">
         <v>5.3</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>0.5</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>1.9</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>7.7</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <v>5.9</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L18" s="3">
+      <c r="M18" s="3">
         <v>6.2</v>
       </c>
-      <c r="M18" s="3">
+      <c r="N18" s="3">
         <v>1.2</v>
       </c>
-      <c r="N18" s="3">
+      <c r="O18" s="3">
         <v>5.9</v>
       </c>
-      <c r="O18" s="3">
+      <c r="P18" s="3">
         <v>3.2</v>
       </c>
-      <c r="P18" s="3">
+      <c r="Q18" s="3">
         <v>2.4</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="R18" s="3">
         <v>1.6</v>
       </c>
-      <c r="R18" s="3">
+      <c r="S18" s="3">
         <v>7.1</v>
       </c>
-      <c r="S18" s="2">
+      <c r="T18" s="2">
         <v>0</v>
       </c>
-      <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
@@ -1582,707 +1674,735 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
-      <c r="AB18" s="8"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="8"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="16">
+        <v>84115</v>
+      </c>
+      <c r="C19" s="4">
         <v>3.6</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>5</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>3.6</v>
       </c>
-      <c r="E19" s="3">
+      <c r="F19" s="3">
         <v>6</v>
       </c>
-      <c r="F19" s="3">
+      <c r="G19" s="3">
         <v>1.7</v>
       </c>
-      <c r="G19" s="3">
+      <c r="H19" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>6.6</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>5.4</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L19" s="3">
         <v>1.8</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M19" s="3">
         <v>6.9</v>
       </c>
-      <c r="M19" s="3">
+      <c r="N19" s="3">
         <v>1</v>
       </c>
-      <c r="N19" s="3">
+      <c r="O19" s="3">
         <v>5.4</v>
       </c>
-      <c r="O19" s="3">
+      <c r="P19" s="3">
         <v>3</v>
       </c>
-      <c r="P19" s="3">
+      <c r="Q19" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R19" s="3">
         <v>1.7</v>
       </c>
-      <c r="R19" s="3">
+      <c r="S19" s="3">
         <v>6.1</v>
       </c>
-      <c r="S19" s="3">
+      <c r="T19" s="3">
         <v>1.6</v>
       </c>
-      <c r="T19" s="2">
+      <c r="U19" s="2">
         <v>0</v>
       </c>
-      <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
-      <c r="AB19" s="8"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="8"/>
     </row>
-    <row r="20" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="16">
+        <v>84111</v>
+      </c>
+      <c r="C20" s="4">
         <v>6.5</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>4.8</v>
       </c>
-      <c r="D20" s="3">
+      <c r="E20" s="3">
         <v>4.3</v>
       </c>
-      <c r="E20" s="3">
+      <c r="F20" s="3">
         <v>10.6</v>
       </c>
-      <c r="F20" s="3">
+      <c r="G20" s="3">
         <v>6.5</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>3.5</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>3.2</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>6.7</v>
       </c>
-      <c r="J20" s="3">
+      <c r="K20" s="3">
         <v>1</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L20" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="L20" s="3">
+      <c r="M20" s="3">
         <v>11.5</v>
       </c>
-      <c r="M20" s="3">
+      <c r="N20" s="3">
         <v>3.7</v>
       </c>
-      <c r="N20" s="3">
+      <c r="O20" s="3">
         <v>1</v>
       </c>
-      <c r="O20" s="3">
+      <c r="P20" s="3">
         <v>6.9</v>
       </c>
-      <c r="P20" s="3">
+      <c r="Q20" s="3">
         <v>6.8</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="R20" s="3">
         <v>6.4</v>
       </c>
-      <c r="R20" s="3">
+      <c r="S20" s="3">
         <v>7.2</v>
       </c>
-      <c r="S20" s="3">
+      <c r="T20" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T20" s="3">
+      <c r="U20" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="U20" s="2">
+      <c r="V20" s="2">
         <v>0</v>
       </c>
-      <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
-      <c r="AB20" s="8"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="8"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="16">
+        <v>84117</v>
+      </c>
+      <c r="C21" s="4">
         <v>1.9</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>9.5</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="3">
         <v>3.3</v>
       </c>
-      <c r="E21" s="3">
+      <c r="F21" s="3">
         <v>5.9</v>
       </c>
-      <c r="F21" s="3">
+      <c r="G21" s="3">
         <v>3.2</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>11.2</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>8.1</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>8.5</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L21" s="3">
         <v>3.8</v>
       </c>
-      <c r="L21" s="3">
+      <c r="M21" s="3">
         <v>6.9</v>
       </c>
-      <c r="M21" s="3">
+      <c r="N21" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="N21" s="3">
+      <c r="O21" s="3">
         <v>8.5</v>
       </c>
-      <c r="O21" s="3">
+      <c r="P21" s="3">
         <v>6.2</v>
       </c>
-      <c r="P21" s="3">
+      <c r="Q21" s="3">
         <v>5.3</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="R21" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="R21" s="3">
+      <c r="S21" s="3">
         <v>10.6</v>
       </c>
-      <c r="S21" s="3">
+      <c r="T21" s="3">
         <v>3</v>
       </c>
-      <c r="T21" s="3">
+      <c r="U21" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="U21" s="3">
+      <c r="V21" s="3">
         <v>7.5</v>
       </c>
-      <c r="V21" s="2">
+      <c r="W21" s="2">
         <v>0</v>
       </c>
-      <c r="W21" s="3"/>
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
-      <c r="AB21" s="8"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="8"/>
     </row>
-    <row r="22" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="16">
+        <v>84117</v>
+      </c>
+      <c r="C22" s="4">
         <v>3.4</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>10.9</v>
       </c>
-      <c r="D22" s="3">
+      <c r="E22" s="3">
         <v>5</v>
       </c>
-      <c r="E22" s="3">
+      <c r="F22" s="3">
         <v>7.4</v>
       </c>
-      <c r="F22" s="3">
+      <c r="G22" s="3">
         <v>5.2</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>6.9</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>12.7</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>10.4</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>10.3</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>5.8</v>
       </c>
-      <c r="L22" s="3">
+      <c r="M22" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="M22" s="3">
+      <c r="N22" s="3">
         <v>6.2</v>
       </c>
-      <c r="N22" s="3">
+      <c r="O22" s="3">
         <v>10.3</v>
       </c>
-      <c r="O22" s="3">
+      <c r="P22" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="P22" s="3">
+      <c r="Q22" s="3">
         <v>7.4</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="R22" s="3">
         <v>6.9</v>
       </c>
-      <c r="R22" s="3">
+      <c r="S22" s="3">
         <v>12</v>
       </c>
-      <c r="S22" s="3">
+      <c r="T22" s="3">
         <v>5</v>
       </c>
-      <c r="T22" s="3">
+      <c r="U22" s="3">
         <v>6.6</v>
       </c>
-      <c r="U22" s="3">
+      <c r="V22" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="V22" s="3">
+      <c r="W22" s="3">
         <v>2</v>
       </c>
-      <c r="W22" s="2">
+      <c r="X22" s="2">
         <v>0</v>
       </c>
-      <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
-      <c r="AB22" s="8"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="8"/>
     </row>
-    <row r="23" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="16">
+        <v>84107</v>
+      </c>
+      <c r="C23" s="4">
         <v>2.4</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D23" s="3">
+      <c r="E23" s="3">
         <v>6.1</v>
       </c>
-      <c r="E23" s="3">
+      <c r="F23" s="3">
         <v>4.7</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>2.5</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>4.2</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <v>10</v>
-      </c>
-      <c r="I23" s="3">
-        <v>7.8</v>
       </c>
       <c r="J23" s="3">
         <v>7.8</v>
       </c>
       <c r="K23" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="L23" s="3">
         <v>4.3</v>
       </c>
-      <c r="L23" s="3">
+      <c r="M23" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="M23" s="3">
+      <c r="N23" s="3">
         <v>3.4</v>
       </c>
-      <c r="N23" s="3">
+      <c r="O23" s="3">
         <v>7.8</v>
       </c>
-      <c r="O23" s="3">
+      <c r="P23" s="3">
         <v>5.5</v>
       </c>
-      <c r="P23" s="3">
+      <c r="Q23" s="3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="R23" s="3">
         <v>4.2</v>
       </c>
-      <c r="R23" s="3">
+      <c r="S23" s="3">
         <v>9.4</v>
       </c>
-      <c r="S23" s="3">
+      <c r="T23" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="T23" s="3">
+      <c r="U23" s="3">
         <v>3.9</v>
       </c>
-      <c r="U23" s="3">
+      <c r="V23" s="3">
         <v>6.8</v>
       </c>
-      <c r="V23" s="3">
+      <c r="W23" s="3">
         <v>2.9</v>
       </c>
-      <c r="W23" s="3">
+      <c r="X23" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="X23" s="2">
+      <c r="Y23" s="2">
         <v>0</v>
       </c>
-      <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
-      <c r="AB23" s="8"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="8"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="16">
+        <v>84118</v>
+      </c>
+      <c r="C24" s="4">
         <v>6.4</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="3">
         <v>6.9</v>
       </c>
-      <c r="D24" s="3">
+      <c r="E24" s="3">
         <v>9.6999999999999993</v>
       </c>
-      <c r="E24" s="3">
+      <c r="F24" s="3">
         <v>0.6</v>
       </c>
-      <c r="F24" s="3">
+      <c r="G24" s="3">
         <v>6</v>
       </c>
-      <c r="G24" s="3">
+      <c r="H24" s="3">
         <v>9</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>4.2</v>
       </c>
-      <c r="J24" s="3">
+      <c r="K24" s="3">
         <v>11.5</v>
       </c>
-      <c r="K24" s="3">
+      <c r="L24" s="3">
         <v>7.8</v>
       </c>
-      <c r="L24" s="3">
+      <c r="M24" s="3">
         <v>0.4</v>
       </c>
-      <c r="M24" s="3">
+      <c r="N24" s="3">
         <v>6.9</v>
       </c>
-      <c r="N24" s="3">
+      <c r="O24" s="3">
         <v>11.5</v>
       </c>
-      <c r="O24" s="3">
+      <c r="P24" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="P24" s="3">
+      <c r="Q24" s="3">
         <v>4.8</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="R24" s="3">
         <v>5.6</v>
       </c>
-      <c r="R24" s="3">
+      <c r="S24" s="3">
         <v>7.5</v>
       </c>
-      <c r="S24" s="3">
+      <c r="T24" s="3">
         <v>5.5</v>
       </c>
-      <c r="T24" s="3">
+      <c r="U24" s="3">
         <v>6.5</v>
       </c>
-      <c r="U24" s="3">
+      <c r="V24" s="3">
         <v>11.4</v>
       </c>
-      <c r="V24" s="3">
+      <c r="W24" s="3">
         <v>6.4</v>
       </c>
-      <c r="W24" s="3">
+      <c r="X24" s="3">
         <v>7.9</v>
       </c>
-      <c r="X24" s="3">
+      <c r="Y24" s="3">
         <v>4.5</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="Z24" s="2">
         <v>0</v>
       </c>
-      <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
-      <c r="AB24" s="8"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="8"/>
     </row>
-    <row r="25" spans="1:28" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="16">
+        <v>84117</v>
+      </c>
+      <c r="C25" s="4">
         <v>2.4</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="3">
         <v>10</v>
       </c>
-      <c r="D25" s="3">
+      <c r="E25" s="3">
         <v>6.1</v>
       </c>
-      <c r="E25" s="3">
+      <c r="F25" s="3">
         <v>6.4</v>
       </c>
-      <c r="F25" s="3">
+      <c r="G25" s="3">
         <v>4.2</v>
       </c>
-      <c r="G25" s="3">
+      <c r="H25" s="3">
         <v>5.9</v>
       </c>
-      <c r="H25" s="3">
+      <c r="I25" s="3">
         <v>11.7</v>
-      </c>
-      <c r="I25" s="3">
-        <v>9.5</v>
       </c>
       <c r="J25" s="3">
         <v>9.5</v>
       </c>
       <c r="K25" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="L25" s="3">
         <v>4.8</v>
       </c>
-      <c r="L25" s="3">
+      <c r="M25" s="3">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M25" s="3">
+      <c r="N25" s="3">
         <v>5.2</v>
       </c>
-      <c r="N25" s="3">
+      <c r="O25" s="3">
         <v>9.5</v>
       </c>
-      <c r="O25" s="3">
+      <c r="P25" s="3">
         <v>7.2</v>
       </c>
-      <c r="P25" s="3">
+      <c r="Q25" s="3">
         <v>6.3</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="R25" s="3">
         <v>5.9</v>
       </c>
-      <c r="R25" s="3">
+      <c r="S25" s="3">
         <v>11.1</v>
       </c>
-      <c r="S25" s="3">
+      <c r="T25" s="3">
         <v>4</v>
       </c>
-      <c r="T25" s="3">
+      <c r="U25" s="3">
         <v>5.6</v>
       </c>
-      <c r="U25" s="3">
+      <c r="V25" s="3">
         <v>8.5</v>
       </c>
-      <c r="V25" s="3">
+      <c r="W25" s="3">
         <v>2.8</v>
       </c>
-      <c r="W25" s="3">
+      <c r="X25" s="3">
         <v>3.4</v>
       </c>
-      <c r="X25" s="3">
+      <c r="Y25" s="3">
         <v>1.7</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Z25" s="3">
         <v>5.4</v>
       </c>
-      <c r="Z25" s="2">
+      <c r="AA25" s="2">
         <v>0</v>
       </c>
-      <c r="AA25" s="3"/>
-      <c r="AB25" s="8"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="8"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="16">
+        <v>84105</v>
+      </c>
+      <c r="C26" s="4">
         <v>5</v>
       </c>
-      <c r="C26" s="3">
+      <c r="D26" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="D26" s="3">
+      <c r="E26" s="3">
         <v>2.8</v>
       </c>
-      <c r="E26" s="3">
+      <c r="F26" s="3">
         <v>10.1</v>
       </c>
-      <c r="F26" s="3">
+      <c r="G26" s="3">
         <v>5.4</v>
       </c>
-      <c r="G26" s="3">
+      <c r="H26" s="3">
         <v>3.5</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <v>6.2</v>
       </c>
-      <c r="J26" s="3">
+      <c r="K26" s="3">
         <v>2.8</v>
       </c>
-      <c r="K26" s="3">
+      <c r="L26" s="3">
         <v>3.2</v>
       </c>
-      <c r="L26" s="3">
+      <c r="M26" s="3">
         <v>11</v>
       </c>
-      <c r="M26" s="3">
+      <c r="N26" s="3">
         <v>3.7</v>
       </c>
-      <c r="N26" s="3">
+      <c r="O26" s="3">
         <v>2.8</v>
       </c>
-      <c r="O26" s="3">
+      <c r="P26" s="3">
         <v>6.4</v>
       </c>
-      <c r="P26" s="3">
+      <c r="Q26" s="3">
         <v>6.5</v>
       </c>
-      <c r="Q26" s="3">
+      <c r="R26" s="3">
         <v>5.7</v>
       </c>
-      <c r="R26" s="3">
+      <c r="S26" s="3">
         <v>6.2</v>
       </c>
-      <c r="S26" s="3">
+      <c r="T26" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="T26" s="3">
+      <c r="U26" s="3">
         <v>4.3</v>
       </c>
-      <c r="U26" s="3">
+      <c r="V26" s="3">
         <v>1.8</v>
       </c>
-      <c r="V26" s="3">
+      <c r="W26" s="3">
         <v>6</v>
       </c>
-      <c r="W26" s="3">
+      <c r="X26" s="3">
         <v>7.9</v>
       </c>
-      <c r="X26" s="3">
+      <c r="Y26" s="3">
         <v>6.8</v>
       </c>
-      <c r="Y26" s="3">
+      <c r="Z26" s="3">
         <v>10.6</v>
       </c>
-      <c r="Z26" s="3">
+      <c r="AA26" s="3">
         <v>7</v>
       </c>
-      <c r="AA26" s="2">
+      <c r="AB26" s="2">
         <v>0</v>
       </c>
-      <c r="AB26" s="8"/>
+      <c r="AC26" s="8"/>
     </row>
-    <row r="27" spans="1:28" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="17">
+        <v>84121</v>
+      </c>
+      <c r="C27" s="9">
         <v>3.6</v>
       </c>
-      <c r="C27" s="10">
+      <c r="D27" s="10">
         <v>13</v>
       </c>
-      <c r="D27" s="10">
+      <c r="E27" s="10">
         <v>7.4</v>
       </c>
-      <c r="E27" s="10">
+      <c r="F27" s="10">
         <v>10.1</v>
       </c>
-      <c r="F27" s="10">
+      <c r="G27" s="10">
         <v>5.5</v>
       </c>
-      <c r="G27" s="10">
+      <c r="H27" s="10">
         <v>7.2</v>
       </c>
-      <c r="H27" s="10">
+      <c r="I27" s="10">
         <v>14.2</v>
       </c>
-      <c r="I27" s="10">
+      <c r="J27" s="10">
         <v>10.7</v>
       </c>
-      <c r="J27" s="10">
+      <c r="K27" s="10">
         <v>14.1</v>
       </c>
-      <c r="K27" s="10">
+      <c r="L27" s="10">
         <v>6</v>
       </c>
-      <c r="L27" s="10">
+      <c r="M27" s="10">
         <v>6.8</v>
       </c>
-      <c r="M27" s="10">
+      <c r="N27" s="10">
         <v>6.4</v>
       </c>
-      <c r="N27" s="10">
+      <c r="O27" s="10">
         <v>14.1</v>
       </c>
-      <c r="O27" s="10">
+      <c r="P27" s="10">
         <v>10.5</v>
       </c>
-      <c r="P27" s="10">
+      <c r="Q27" s="10">
         <v>8.8000000000000007</v>
       </c>
-      <c r="Q27" s="10">
+      <c r="R27" s="10">
         <v>8.4</v>
       </c>
-      <c r="R27" s="10">
+      <c r="S27" s="10">
         <v>13.6</v>
       </c>
-      <c r="S27" s="10">
+      <c r="T27" s="10">
         <v>5.2</v>
       </c>
-      <c r="T27" s="10">
+      <c r="U27" s="10">
         <v>6.9</v>
       </c>
-      <c r="U27" s="10">
+      <c r="V27" s="10">
         <v>13.1</v>
       </c>
-      <c r="V27" s="10">
+      <c r="W27" s="10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="W27" s="10">
+      <c r="X27" s="10">
         <v>4.7</v>
       </c>
-      <c r="X27" s="10">
+      <c r="Y27" s="10">
         <v>3.1</v>
       </c>
-      <c r="Y27" s="10">
+      <c r="Z27" s="10">
         <v>7.8</v>
       </c>
-      <c r="Z27" s="10">
+      <c r="AA27" s="10">
         <v>1.3</v>
       </c>
-      <c r="AA27" s="10">
+      <c r="AB27" s="10">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AB27" s="11">
+      <c r="AC27" s="11">
         <v>0</v>
       </c>
     </row>
@@ -2293,6 +2413,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2802,15 +2931,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2861,6 +2981,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2876,14 +3004,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
created nearest neighbor algorithm
</commit_message>
<xml_diff>
--- a/data/WGUPS Distance Table.xlsx
+++ b/data/WGUPS Distance Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\PycharmProjects\DSAII\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E84C1E9-D498-48DA-A7BF-C629DE07A583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2108F4D4-5664-4871-A128-3D0EB5DDFE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-23" windowWidth="21795" windowHeight="12976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
   <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,15 +2413,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="51" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dca2bb0f68bdf94cc5f80c9292ca56b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d4cb8629785915e947a4406c57312ba8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2931,6 +2922,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2981,14 +2981,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346B5534-CC83-47DD-8523-BB97FB1B43B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3004,6 +2996,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>